<commit_message>
BLEU calculated for grouped results
</commit_message>
<xml_diff>
--- a/new_results.xlsx
+++ b/new_results.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bleu Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -462,6 +467,9 @@
       <c r="C2" t="n">
         <v>12</v>
       </c>
+      <c r="D2" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -475,6 +483,9 @@
       <c r="C3" t="n">
         <v>4.509141633167239</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.3379800452414116</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -488,6 +499,9 @@
       <c r="C4" t="n">
         <v>0.2519836364707003</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.06163144718522491</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -501,6 +515,9 @@
       <c r="C5" t="n">
         <v>4.187896660234053</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.2526101718712371</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -514,6 +531,9 @@
       <c r="C6" t="n">
         <v>4.226159505270275</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.3001221066198977</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -527,6 +547,9 @@
       <c r="C7" t="n">
         <v>4.56091283323509</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.318314367467799</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -540,6 +563,9 @@
       <c r="C8" t="n">
         <v>4.668491763737882</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.4003414786054609</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -552,6 +578,9 @@
       </c>
       <c r="C9" t="n">
         <v>4.850476179074347</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.4234614838907227</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +594,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,6 +613,11 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bleu Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -597,6 +631,9 @@
       <c r="C2" t="n">
         <v>18</v>
       </c>
+      <c r="D2" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -610,6 +647,9 @@
       <c r="C3" t="n">
         <v>5.01797187808681</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.2333973274164544</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -623,6 +663,9 @@
       <c r="C4" t="n">
         <v>0.2418078243901703</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.06010737819688104</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -636,6 +679,9 @@
       <c r="C5" t="n">
         <v>4.727530209210354</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.1613445191462458</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -649,6 +695,9 @@
       <c r="C6" t="n">
         <v>4.834031464161255</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.1864222185487955</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -662,6 +711,9 @@
       <c r="C7" t="n">
         <v>4.972781833884827</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.2200177007161382</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -675,6 +727,9 @@
       <c r="C8" t="n">
         <v>5.080620388748667</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.2586572081769725</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -687,6 +742,9 @@
       </c>
       <c r="C9" t="n">
         <v>5.442023715745888</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3755414285120398</v>
       </c>
     </row>
   </sheetData>
@@ -700,7 +758,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -719,6 +777,11 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bleu Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -732,6 +795,9 @@
       <c r="C2" t="n">
         <v>12</v>
       </c>
+      <c r="D2" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -745,6 +811,9 @@
       <c r="C3" t="n">
         <v>4.598723040890902</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.3100629579914316</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -758,6 +827,9 @@
       <c r="C4" t="n">
         <v>0.2627783201038496</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.05427818329692558</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -771,6 +843,9 @@
       <c r="C5" t="n">
         <v>4.274803438248017</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.2342854631721591</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -784,6 +859,9 @@
       <c r="C6" t="n">
         <v>4.282698730529348</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.274795500128002</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -797,6 +875,9 @@
       <c r="C7" t="n">
         <v>4.65141397015169</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.2910296028794263</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -810,6 +891,9 @@
       <c r="C8" t="n">
         <v>4.780756512580369</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.3660807916788333</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -822,6 +906,9 @@
       </c>
       <c r="C9" t="n">
         <v>4.951251820766528</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3926788350602298</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -854,6 +941,11 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bleu Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -867,6 +959,9 @@
       <c r="C2" t="n">
         <v>36</v>
       </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -880,6 +975,9 @@
       <c r="C3" t="n">
         <v>5.097010301046057</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.2139060874527758</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -893,6 +991,9 @@
       <c r="C4" t="n">
         <v>0.2564186101664079</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.05289529993101381</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -906,6 +1007,9 @@
       <c r="C5" t="n">
         <v>4.762326063866308</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.1449004311910021</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -919,6 +1023,9 @@
       <c r="C6" t="n">
         <v>4.882817609331781</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.1726456028111074</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -932,6 +1039,9 @@
       <c r="C7" t="n">
         <v>5.034241604636328</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.2018272405865633</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -945,6 +1055,9 @@
       <c r="C8" t="n">
         <v>5.230141017033226</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.2377500036178558</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -957,6 +1070,9 @@
       </c>
       <c r="C9" t="n">
         <v>5.58593210710479</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3452394241528321</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +1086,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -989,6 +1105,11 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bleu Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1002,6 +1123,9 @@
       <c r="C2" t="n">
         <v>36</v>
       </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1015,6 +1139,9 @@
       <c r="C3" t="n">
         <v>4.686341819629901</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.2959787316499679</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1028,6 +1155,9 @@
       <c r="C4" t="n">
         <v>0.2343528750295514</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.05558229146353377</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1041,6 +1171,9 @@
       <c r="C5" t="n">
         <v>4.304973932859437</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.2105900010616825</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1054,6 +1187,9 @@
       <c r="C6" t="n">
         <v>4.463663668282909</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.2540433220025421</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1067,6 +1203,9 @@
       <c r="C7" t="n">
         <v>4.761710256553151</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.286640315541796</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1080,6 +1219,9 @@
       <c r="C8" t="n">
         <v>4.886758501318674</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.3479801045752431</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1092,6 +1234,9 @@
       </c>
       <c r="C9" t="n">
         <v>4.967797730617554</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3948788672519359</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1250,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1124,6 +1269,11 @@
           <t>Euclidean Distance</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Bleu Score</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1137,6 +1287,9 @@
       <c r="C2" t="n">
         <v>36</v>
       </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1150,6 +1303,9 @@
       <c r="C3" t="n">
         <v>5.09701031445598</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.2133887891892107</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1163,6 +1319,9 @@
       <c r="C4" t="n">
         <v>0.2564186666748767</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.05674817867384331</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1176,6 +1335,9 @@
       <c r="C5" t="n">
         <v>4.762326107438171</v>
       </c>
+      <c r="D5" t="n">
+        <v>0.14007740193289</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1189,6 +1351,9 @@
       <c r="C6" t="n">
         <v>4.882817527186092</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.1787050173166828</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1202,6 +1367,9 @@
       <c r="C7" t="n">
         <v>5.034241824466493</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.2003626985101559</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1215,6 +1383,9 @@
       <c r="C8" t="n">
         <v>5.230141426680463</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.2289875544707819</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1227,6 +1398,9 @@
       </c>
       <c r="C9" t="n">
         <v>5.58593122676529</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.3593458407653583</v>
       </c>
     </row>
   </sheetData>

</xml_diff>